<commit_message>
research ended part 2 413
</commit_message>
<xml_diff>
--- a/TERM3/T3B2-ICTNPL413-Evaluate_net_regulations_legislation_telecommunications_industry/2-ICTNPL413-Assessment_Task 2/Assessmet-questions/ICTNPL413_AssessmentTask_Manuel_S_Perez_E-ASSESS-INFORMATION.xlsx
+++ b/TERM3/T3B2-ICTNPL413-Evaluate_net_regulations_legislation_telecommunications_industry/2-ICTNPL413-Assessment_Task 2/Assessmet-questions/ICTNPL413_AssessmentTask_Manuel_S_Perez_E-ASSESS-INFORMATION.xlsx
@@ -7,6 +7,7 @@
     <sheet state="visible" name="Industry" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="economyXtelcos" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="SUM-Assess" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Eval-report-comparison" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="123">
   <si>
     <t>Economic factors that can affect growth</t>
   </si>
@@ -357,6 +358,9 @@
     <t>Imposes carrier licence obligations on large companies. It establishes the framework for network facility access and interconnection with other carriers' networks. It also contains section 313, which can be used by government agencies to request carriers take action to prevent criminal activity.</t>
   </si>
   <si>
+    <t>the universal access and competition policy has transformed the market. Driven by the principle that essential services should be accessible to all, the government created the National Broadband Network (NBN), a public company. The NBN operates as a wholesale provider, requiring retail companies to use its infrastructure, which has restructured the market and fostered competition at the service level. The ACCC complements this policy by regulating access to other operators' networks to prevent monopolies and ensure prices remain competitive for consumers.</t>
+  </si>
+  <si>
     <t>Regulates the Universal Service Obligation (USO), which requires the primary carrier (Telstra) to provide a standard telephone service and payphones to all Australians, regardless of location. Large companies must also contribute to the Telecommunications Industry Levy to fund these services.</t>
   </si>
   <si>
@@ -372,9 +376,7 @@
     <t>Applies to large companies to regulate competition. The ACCC uses its powers under this Act to prevent anti-competitive conduct, regulate access to essential network infrastructure, and oversee compliance with consumer protection laws.</t>
   </si>
   <si>
-    <t xml:space="preserve">Consumer Protection: 
-Both the ACCC and ACMA have increased their focus on protecting consumers from issues like scams, misleading advertising, and unfair sales practices. This includes issuing hefty penalties, like the $100 million penalty Optus agreed to pay for unconscionable conduct in selling products con-sumers did not need.
-</t>
+    <t>consumer protection is another important driver. Regulatory bodies such as the ACCC (Australian Competition and Consumer Commission) and the ACMA (Australian Communications and Media Authority) operate with a political mandate to protect citizens from practices such as scams, misleading advertising, and unfair selling. These bodies have the authority to impose significant financial penalties, such as the $100 million fine Optus was forced to pay for misconduct, demonstrating the government's seriousness in this area.</t>
   </si>
   <si>
     <t>Imposes obligations on large companies that also operate broadcasting or subscription television services, such as rules on media ownership and content diversity.</t>
@@ -386,13 +388,7 @@
     <t>Requires large companies handling personal data to comply with the Australian Privacy Principles (APPs). This includes a mandatory data breach notification scheme and taking reasonable steps to secure personal information.</t>
   </si>
   <si>
-    <t xml:space="preserve">Security:
-The government created the "Cyber Security Act 2024" in response to the lack of a legal framework for cybersecurity.
-Between 2022 and 2023, the data theft scandals that rocked the country highlighted the lack of legal measures to respond to cybercriminals. In 2022, Optus suffered an attack that allowed the personal data of 40% of the population to be published. That same year, Medibank suffered a ransomware attack that compromised the personal data of 9.7 million people, resulting in the data being leaked to the dark web after the ransom was not received. Finally, in 2023, Latitude Financial suffered an attack that exposed the personal data of 14 million people online.
-Prior to the Cyber Security Act, the legal framework was provided by the Privacy Act 1988, on the protection of personal data, and the Security of Critical Infrastructure Act 2018, on the protection of critical sectors for the country. Despite the existence of these laws, there were no laws regarding the legal obligations of companies.
-The Cyber Security Act requires companies to report serious cybersecurity incidents and report ransom demands starting May 30 of this year. This response to cyber extortion also increased fines for security breaches from 2.2 million to 50 million, or more as determined by law.
-In short, the law was created to protect Australians' data, increase transparency in the face of cyberattack incidents, and strengthen national resilience to cyber threats.
-</t>
+    <t>cybersecurity has become a political priority. Following a series of large-scale data breaches at companies such as Optus and Medibank between 2022 and 2023, the Australian government responded with the Cybersecurity Act of 2024. This legislation has directly impacted companies by requiring them to report serious incidents and ransom demands, increasing their liability. Furthermore, it has dramatically increased fines for security breaches, creating a strong incentive for companies to invest in stronger protection of their customers' data.</t>
   </si>
   <si>
     <t>Imposes obligations on large social media platforms and internet service providers to address cyberbullying and harmful content. The eSafety Commissioner can issue removal notices to these companies.</t>
@@ -406,12 +402,84 @@
   <si>
     <t>Imposes responsibilities on telecommunications companies to combat copyright infringement. It is often used to issue court orders to block websites that facilitate piracy.</t>
   </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Summary Report</t>
+  </si>
+  <si>
+    <t>Comprehensive Report</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>To provide a quick, high-level overview.</t>
+  </si>
+  <si>
+    <t>To offer a detailed, in-depth analysis.</t>
+  </si>
+  <si>
+    <t>Audience</t>
+  </si>
+  <si>
+    <t>Executives, managers, and time-poor decision-makers.</t>
+  </si>
+  <si>
+    <t>Technical staff, researchers, and stakeholders who need all the nitty-gritty details.</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Typically 3 to 7 pages.</t>
+  </si>
+  <si>
+    <t>Generally 15 to 50+ pages.</t>
+  </si>
+  <si>
+    <t>Level of Detail</t>
+  </si>
+  <si>
+    <t>Low. Focuses on the most critical points.</t>
+  </si>
+  <si>
+    <t>High. Includes detailed data, methodology, and thorough analysis.</t>
+  </si>
+  <si>
+    <t>Key Content</t>
+  </si>
+  <si>
+    <t>Executive summary, key findings, core conclusions, and main recommendations.</t>
+  </si>
+  <si>
+    <t>All sections of a formal report: detailed introduction, methodology, full findings, conclusions, recommendations, lessons learned, limitations, and appendices.</t>
+  </si>
+  <si>
+    <t>Primary Use</t>
+  </si>
+  <si>
+    <t>For swift, efficient decision-making.</t>
+  </si>
+  <si>
+    <t>For transparency, accountability, and a deep understanding of the project.</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Concise, using bullet points or short paragraphs.</t>
+  </si>
+  <si>
+    <t>Structured with multiple sections and subheadings, often with charts and graphs.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -511,6 +579,17 @@
       <sz val="11.0"/>
       <color rgb="FF1B1C1D"/>
       <name val="Google Sans Text"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="14">
@@ -643,7 +722,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -768,10 +847,13 @@
     <xf borderId="1" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="12" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="12" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -779,9 +861,6 @@
     </xf>
     <xf borderId="1" fillId="11" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="13" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -794,6 +873,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -816,6 +901,10 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -4863,9 +4952,10 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="29.63"/>
-    <col customWidth="1" min="3" max="3" width="35.75"/>
-    <col customWidth="1" min="4" max="4" width="80.25"/>
+    <col customWidth="1" min="1" max="1" width="24.38"/>
+    <col customWidth="1" min="2" max="2" width="78.0"/>
+    <col customWidth="1" min="3" max="3" width="81.13"/>
+    <col customWidth="1" min="4" max="4" width="101.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5144,7 +5234,9 @@
       <c r="C10" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="48"/>
+      <c r="D10" s="48" t="s">
+        <v>84</v>
+      </c>
       <c r="E10" s="37"/>
       <c r="F10" s="37"/>
       <c r="G10" s="37"/>
@@ -5176,9 +5268,9 @@
         <v>45</v>
       </c>
       <c r="C11" s="47" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
-      <c r="D11" s="48"/>
+      <c r="D11" s="50"/>
       <c r="E11" s="37"/>
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
@@ -5210,9 +5302,9 @@
         <v>47</v>
       </c>
       <c r="C12" s="47" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
-      <c r="D12" s="48"/>
+      <c r="D12" s="50"/>
       <c r="E12" s="37"/>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
@@ -5244,9 +5336,9 @@
         <v>49</v>
       </c>
       <c r="C13" s="47" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
-      <c r="D13" s="48"/>
+      <c r="D13" s="50"/>
       <c r="E13" s="37"/>
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
@@ -5271,16 +5363,16 @@
       <c r="Z13" s="37"/>
     </row>
     <row r="14">
-      <c r="A14" s="50" t="s">
+      <c r="A14" s="51" t="s">
         <v>50</v>
       </c>
       <c r="B14" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="51" t="s">
-        <v>87</v>
+      <c r="C14" s="52" t="s">
+        <v>88</v>
       </c>
-      <c r="D14" s="48"/>
+      <c r="D14" s="50"/>
       <c r="E14" s="37"/>
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
@@ -5311,11 +5403,11 @@
       <c r="B15" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="51" t="s">
-        <v>88</v>
+      <c r="C15" s="52" t="s">
+        <v>89</v>
       </c>
-      <c r="D15" s="52" t="s">
-        <v>89</v>
+      <c r="D15" s="48" t="s">
+        <v>90</v>
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="37"/>
@@ -5348,7 +5440,7 @@
         <v>55</v>
       </c>
       <c r="C16" s="47" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D16" s="53"/>
       <c r="E16" s="37"/>
@@ -5382,7 +5474,7 @@
         <v>57</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D17" s="53"/>
       <c r="E17" s="37"/>
@@ -5416,10 +5508,10 @@
         <v>59</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
-      <c r="D18" s="52" t="s">
-        <v>93</v>
+      <c r="D18" s="48" t="s">
+        <v>94</v>
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="37"/>
@@ -5445,14 +5537,14 @@
       <c r="Z18" s="37"/>
     </row>
     <row r="19">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="51" t="s">
         <v>60</v>
       </c>
       <c r="B19" s="55" t="s">
         <v>61</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D19" s="53"/>
       <c r="E19" s="37"/>
@@ -5479,14 +5571,14 @@
       <c r="Z19" s="37"/>
     </row>
     <row r="20">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="51" t="s">
         <v>62</v>
       </c>
       <c r="B20" s="55" t="s">
         <v>63</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D20" s="53"/>
       <c r="E20" s="37"/>
@@ -5513,14 +5605,14 @@
       <c r="Z20" s="37"/>
     </row>
     <row r="21">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="51" t="s">
         <v>64</v>
       </c>
       <c r="B21" s="49" t="s">
         <v>65</v>
       </c>
       <c r="C21" s="54" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D21" s="53"/>
       <c r="E21" s="37"/>
@@ -5547,14 +5639,14 @@
       <c r="Z21" s="37"/>
     </row>
     <row r="22">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="51" t="s">
         <v>66</v>
       </c>
       <c r="B22" s="49" t="s">
         <v>67</v>
       </c>
       <c r="C22" s="47" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D22" s="53"/>
       <c r="E22" s="37"/>
@@ -33191,4 +33283,111 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="30.88"/>
+    <col customWidth="1" min="3" max="3" width="46.88"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="58" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="58" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="58" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="58" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="58" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="58" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>